<commit_message>
update test.xlsx file. final format
</commit_message>
<xml_diff>
--- a/packages/web/test.xlsx
+++ b/packages/web/test.xlsx
@@ -26,7 +26,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="E3" authorId="0">
+    <comment ref="C3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -39,7 +39,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0">
+    <comment ref="C4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +57,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+  <si>
+    <t xml:space="preserve">cols/session</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date initialized</t>
+  </si>
   <si>
     <t xml:space="preserve">experiment title</t>
   </si>
@@ -65,25 +71,28 @@
     <t xml:space="preserve">Addiction Study 12</t>
   </si>
   <si>
+    <t xml:space="preserve">last updated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num static identifiers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num treatments</t>
+  </si>
+  <si>
     <t xml:space="preserve">primary experimenter</t>
   </si>
   <si>
     <t xml:space="preserve">Quinn</t>
   </si>
   <si>
-    <t xml:space="preserve">date initialized</t>
-  </si>
-  <si>
-    <t xml:space="preserve">last updated</t>
-  </si>
-  <si>
     <t xml:space="preserve">total sessions</t>
   </si>
   <si>
-    <t xml:space="preserve">cols/session</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num treatments</t>
+    <t xml:space="preserve">treatments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h2o, EtOH</t>
   </si>
   <si>
     <t xml:space="preserve">Session 1</t>
@@ -92,10 +101,7 @@
     <t xml:space="preserve">Session 2</t>
   </si>
   <si>
-    <t xml:space="preserve">RatID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Experimental Condition</t>
+    <t xml:space="preserve">Session 3</t>
   </si>
   <si>
     <t xml:space="preserve">RackID</t>
@@ -104,7 +110,7 @@
     <t xml:space="preserve">CageID</t>
   </si>
   <si>
-    <t xml:space="preserve">body weight</t>
+    <t xml:space="preserve">is Dummy</t>
   </si>
   <si>
     <t xml:space="preserve">pre (h2o)</t>
@@ -117,15 +123,6 @@
   </si>
   <si>
     <t xml:space="preserve">post (EtOH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0xFFFFFF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Warm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cool</t>
   </si>
 </sst>
 </file>
@@ -201,7 +198,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -212,6 +209,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -237,43 +238,43 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>3</v>
+      <c r="B2" s="1" t="n">
+        <v>1571544000000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>1571544000000</v>
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>1581624044775</v>
@@ -281,34 +282,43 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>30</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="B7" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="0" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="3"/>
+      <c r="A8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1"/>
-      <c r="B9" s="3"/>
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -326,13 +336,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M4" activeCellId="0" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.46"/>
@@ -347,34 +357,37 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F1" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>10</v>
+      <c r="D1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>18</v>
@@ -383,10 +396,10 @@
         <v>19</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>18</v>
@@ -394,165 +407,155 @@
       <c r="M2" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="N2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="0" t="n">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="F3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="B4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="C4" s="4" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="C5" s="4" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="J3" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="M3" s="0" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="L4" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="M4" s="0" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="K5" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="L5" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="M5" s="0" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>2</v>
+      <c r="C6" s="4" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>600</v>
+        <v>26</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>26</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="I6" s="0" t="n">
         <v>28</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update comments in test excel file
</commit_message>
<xml_diff>
--- a/packages/web/test.xlsx
+++ b/packages/web/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -35,7 +35,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">A comment on E3</t>
+          <t xml:space="preserve">A comment on C3</t>
         </r>
       </text>
     </comment>
@@ -48,7 +48,8 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">A comment on E3</t>
+          <t xml:space="preserve">A comment on C4
+</t>
         </r>
       </text>
     </comment>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t xml:space="preserve">date initialized</t>
   </si>
@@ -117,9 +118,6 @@
   </si>
   <si>
     <t xml:space="preserve">post (EtOH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kkkjjj</t>
   </si>
 </sst>
 </file>
@@ -242,11 +240,11 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.46"/>
@@ -326,11 +324,11 @@
   </sheetPr>
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M4" activeCellId="0" sqref="M4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.46"/>
@@ -485,9 +483,6 @@
       <c r="K4" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="M4" s="0" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">

</xml_diff>

<commit_message>
make xlsx parser account for pre but no post
</commit_message>
<xml_diff>
--- a/packages/web/test.xlsx
+++ b/packages/web/test.xlsx
@@ -244,7 +244,7 @@
       <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.46"/>
@@ -325,10 +325,10 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.46"/>
@@ -537,12 +537,6 @@
       <c r="E6" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="F6" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>28</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
update test.xlsx so it can test sessions without post weights
</commit_message>
<xml_diff>
--- a/packages/web/test.xlsx
+++ b/packages/web/test.xlsx
@@ -244,7 +244,7 @@
       <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.46"/>
@@ -325,10 +325,10 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.46"/>

</xml_diff>

<commit_message>
update test.xlsx to include a cage with no sessions
</commit_message>
<xml_diff>
--- a/packages/web/test.xlsx
+++ b/packages/web/test.xlsx
@@ -244,7 +244,7 @@
       <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.46"/>
@@ -322,13 +322,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.46"/>
@@ -538,6 +538,17 @@
         <v>26</v>
       </c>
     </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
update test.xlsx to include a cage with all of its session completed
</commit_message>
<xml_diff>
--- a/packages/web/test.xlsx
+++ b/packages/web/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -240,11 +240,11 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.46"/>
@@ -295,7 +295,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>30</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -324,11 +324,11 @@
   </sheetPr>
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.46"/>
@@ -545,7 +545,8 @@
       <c r="B7" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C7" s="4" t="b">
+      <c r="C7" s="4" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>